<commit_message>
updated class and id map spreadsheet
</commit_message>
<xml_diff>
--- a/assets/Class and Id Map.xlsx
+++ b/assets/Class and Id Map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>Small</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Parent  div to return results from API call. This div is hidden until return comes back from API. Build 10 of these using jQuery for each return</t>
+  </si>
+  <si>
+    <t>Radio button temporarily implemented for functionality</t>
   </si>
 </sst>
 </file>
@@ -609,7 +612,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,7 +719,9 @@
       <c r="D7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
@@ -729,7 +734,9 @@
       <c r="D8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
@@ -742,7 +749,9 @@
       <c r="D9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
@@ -757,7 +766,9 @@
       <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
@@ -770,7 +781,9 @@
       <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
@@ -783,7 +796,9 @@
       <c r="D12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
@@ -796,7 +811,9 @@
       <c r="D13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">

</xml_diff>